<commit_message>
removed summary statistics calculation following science review minor updates to gitignore and library following review
</commit_message>
<xml_diff>
--- a/ref/MPStarter1_0.xlsx
+++ b/ref/MPStarter1_0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\003_Bachelor_Master_PhD_PostDoc\04_Masterarbeiten\2021_Joey_O'Dell_MA\002_Data\003_Code\ref\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Congo\reclarify\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB50B4B-BBC2-46FE-9F0A-6E162B778FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11460"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MPStarter1_0" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="163">
   <si>
     <t>Grouping</t>
   </si>
@@ -505,12 +506,15 @@
   </si>
   <si>
     <t>Congo_typical_matrix_4</t>
+  </si>
+  <si>
+    <t>PET_20_63µm_MPstarter_20_11_19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1329,11 +1333,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B142"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="D141" sqref="D141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2478,8 +2482,16 @@
         <v>142</v>
       </c>
     </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>162</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:B142">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B142">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>